<commit_message>
further design fig work
</commit_message>
<xml_diff>
--- a/data/design.dat.xlsx
+++ b/data/design.dat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kristili\R\ribose-paper\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B43A3FF-52A9-4F25-A0ED-28154963E206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E5F02F-92F8-4A6B-9390-DC002DD86204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{51A3D02E-D8FD-4892-BC71-924420679D87}"/>
   </bookViews>
@@ -393,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{296EA4C1-7D9C-4FB0-9EA6-62671A855520}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:B23"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -411,7 +411,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -419,7 +419,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -427,7 +427,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -435,7 +435,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -443,7 +443,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -451,7 +451,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -459,7 +459,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B8">
         <v>6</v>
@@ -467,7 +467,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B9">
         <v>7</v>
@@ -475,7 +475,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B10">
         <v>8</v>
@@ -483,7 +483,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B11">
         <v>9</v>
@@ -491,10 +491,122 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B12">
         <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>9</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>11</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>12</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>13</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>14</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>15</v>
+      </c>
+      <c r="B20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>16</v>
+      </c>
+      <c r="B21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>17</v>
+      </c>
+      <c r="B22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>18</v>
+      </c>
+      <c r="B23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>19</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>20</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>21</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>